<commit_message>
implemented and tested single step evaluation
</commit_message>
<xml_diff>
--- a/ACEBench/score_all/score_en/result.xlsx
+++ b/ACEBench/score_all/score_en/result.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA2"/>
+  <dimension ref="A1:AA3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -646,6 +646,91 @@
         <v>0.833</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>gpt-4o-2024-05-13</t>
+        </is>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>0.86</v>
+      </c>
+      <c r="G3" s="1" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="H3" s="1" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="I3" s="1" t="n">
+        <v>0.87</v>
+      </c>
+      <c r="J3" s="1" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="K3" s="1" t="n">
+        <v>0.895</v>
+      </c>
+      <c r="L3" s="1" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="M3" s="1" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="N3" s="1" t="n">
+        <v>0.64</v>
+      </c>
+      <c r="O3" s="1" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="P3" s="1" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="Q3" s="1" t="n">
+        <v>0.861</v>
+      </c>
+      <c r="R3" s="1" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="S3" s="1" t="n">
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="T3" s="1" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="U3" s="1" t="n">
+        <v>0.907</v>
+      </c>
+      <c r="V3" s="1" t="n">
+        <v>0.367</v>
+      </c>
+      <c r="W3" s="1" t="n">
+        <v>0.6830000000000001</v>
+      </c>
+      <c r="X3" s="1" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="Y3" s="1" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="Z3" s="1" t="n">
+        <v>0.384</v>
+      </c>
+      <c r="AA3" s="1" t="n">
+        <v>0.8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
successfully made the multi turn agent to perform normally
</commit_message>
<xml_diff>
--- a/ACEBench/score_all/score_en/result.xlsx
+++ b/ACEBench/score_all/score_en/result.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA3"/>
+  <dimension ref="A1:AA4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -564,11 +564,11 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>gpt-4o</t>
+          <t>gpt-4.1</t>
         </is>
       </c>
       <c r="B2" s="1" t="n">
-        <v>0.96</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>0.98</v>
@@ -577,43 +577,43 @@
         <v>1</v>
       </c>
       <c r="E2" s="1" t="n">
-        <v>0.96</v>
+        <v>0.9</v>
       </c>
       <c r="F2" s="1" t="n">
-        <v>0.88</v>
+        <v>0.9</v>
       </c>
       <c r="G2" s="1" t="n">
-        <v>0.98</v>
+        <v>1</v>
       </c>
       <c r="H2" s="1" t="n">
-        <v>0.96</v>
+        <v>0.953</v>
       </c>
       <c r="I2" s="1" t="n">
-        <v>0.96</v>
+        <v>0.91</v>
       </c>
       <c r="J2" s="1" t="n">
-        <v>0.85</v>
+        <v>0.89</v>
       </c>
       <c r="K2" s="1" t="n">
-        <v>0.905</v>
+        <v>0.9</v>
       </c>
       <c r="L2" s="1" t="n">
-        <v>0.68</v>
+        <v>0.64</v>
       </c>
       <c r="M2" s="1" t="n">
         <v>0.64</v>
       </c>
       <c r="N2" s="1" t="n">
-        <v>0.66</v>
+        <v>0.64</v>
       </c>
       <c r="O2" s="1" t="n">
-        <v>0.82</v>
+        <v>0.76</v>
       </c>
       <c r="P2" s="1" t="n">
-        <v>0.74</v>
+        <v>0.8</v>
       </c>
       <c r="Q2" s="1" t="n">
-        <v>0.871</v>
+        <v>0.863</v>
       </c>
       <c r="R2" s="1" t="n">
         <v>0.9</v>
@@ -622,86 +622,86 @@
         <v>0.9399999999999999</v>
       </c>
       <c r="T2" s="1" t="n">
-        <v>0.96</v>
+        <v>0.88</v>
       </c>
       <c r="U2" s="1" t="n">
-        <v>0.9330000000000001</v>
+        <v>0.907</v>
       </c>
       <c r="V2" s="1" t="n">
-        <v>0.433</v>
+        <v>0.5669999999999999</v>
       </c>
       <c r="W2" s="1" t="n">
-        <v>0.753</v>
+        <v>0.746</v>
       </c>
       <c r="X2" s="1" t="n">
-        <v>0.6</v>
+        <v>0.95</v>
       </c>
       <c r="Y2" s="1" t="n">
-        <v>0.77</v>
+        <v>0.958</v>
       </c>
       <c r="Z2" s="1" t="n">
-        <v>0.516</v>
+        <v>0.758</v>
       </c>
       <c r="AA2" s="1" t="n">
-        <v>0.833</v>
+        <v>0.859</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>gpt-4o-2024-05-13</t>
+          <t>gpt-4o</t>
         </is>
       </c>
       <c r="B3" s="1" t="n">
         <v>0.96</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>0.96</v>
+        <v>0.98</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E3" s="1" t="n">
-        <v>0.9399999999999999</v>
+        <v>0.96</v>
       </c>
       <c r="F3" s="1" t="n">
-        <v>0.86</v>
+        <v>0.88</v>
       </c>
       <c r="G3" s="1" t="n">
         <v>0.98</v>
       </c>
       <c r="H3" s="1" t="n">
-        <v>0.95</v>
+        <v>0.96</v>
       </c>
       <c r="I3" s="1" t="n">
-        <v>0.87</v>
+        <v>0.96</v>
       </c>
       <c r="J3" s="1" t="n">
-        <v>0.92</v>
+        <v>0.85</v>
       </c>
       <c r="K3" s="1" t="n">
-        <v>0.895</v>
+        <v>0.905</v>
       </c>
       <c r="L3" s="1" t="n">
         <v>0.68</v>
       </c>
       <c r="M3" s="1" t="n">
-        <v>0.6</v>
+        <v>0.64</v>
       </c>
       <c r="N3" s="1" t="n">
-        <v>0.64</v>
+        <v>0.66</v>
       </c>
       <c r="O3" s="1" t="n">
-        <v>0.8</v>
+        <v>0.82</v>
       </c>
       <c r="P3" s="1" t="n">
-        <v>0.76</v>
+        <v>0.74</v>
       </c>
       <c r="Q3" s="1" t="n">
-        <v>0.861</v>
+        <v>0.871</v>
       </c>
       <c r="R3" s="1" t="n">
-        <v>0.82</v>
+        <v>0.9</v>
       </c>
       <c r="S3" s="1" t="n">
         <v>0.9399999999999999</v>
@@ -710,24 +710,109 @@
         <v>0.96</v>
       </c>
       <c r="U3" s="1" t="n">
+        <v>0.9330000000000001</v>
+      </c>
+      <c r="V3" s="1" t="n">
+        <v>0.433</v>
+      </c>
+      <c r="W3" s="1" t="n">
+        <v>0.753</v>
+      </c>
+      <c r="X3" s="1" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="Y3" s="1" t="n">
+        <v>0.77</v>
+      </c>
+      <c r="Z3" s="1" t="n">
+        <v>0.516</v>
+      </c>
+      <c r="AA3" s="1" t="n">
+        <v>0.833</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>gpt-4o-2024-05-13</t>
+        </is>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>0.86</v>
+      </c>
+      <c r="G4" s="1" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="H4" s="1" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="I4" s="1" t="n">
+        <v>0.87</v>
+      </c>
+      <c r="J4" s="1" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="K4" s="1" t="n">
+        <v>0.895</v>
+      </c>
+      <c r="L4" s="1" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="M4" s="1" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="N4" s="1" t="n">
+        <v>0.64</v>
+      </c>
+      <c r="O4" s="1" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="P4" s="1" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="Q4" s="1" t="n">
+        <v>0.861</v>
+      </c>
+      <c r="R4" s="1" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="S4" s="1" t="n">
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="T4" s="1" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="U4" s="1" t="n">
         <v>0.907</v>
       </c>
-      <c r="V3" s="1" t="n">
+      <c r="V4" s="1" t="n">
         <v>0.367</v>
       </c>
-      <c r="W3" s="1" t="n">
+      <c r="W4" s="1" t="n">
         <v>0.6830000000000001</v>
       </c>
-      <c r="X3" s="1" t="n">
+      <c r="X4" s="1" t="n">
         <v>0.4</v>
       </c>
-      <c r="Y3" s="1" t="n">
+      <c r="Y4" s="1" t="n">
         <v>0.57</v>
       </c>
-      <c r="Z3" s="1" t="n">
+      <c r="Z4" s="1" t="n">
         <v>0.384</v>
       </c>
-      <c r="AA3" s="1" t="n">
+      <c r="AA4" s="1" t="n">
         <v>0.8</v>
       </c>
     </row>

</xml_diff>